<commit_message>
added chimera-corrected cvrg as column
</commit_message>
<xml_diff>
--- a/tools/test-data/Variant_Analyzer_test.xlsx
+++ b/tools/test-data/Variant_Analyzer_test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1456" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1458" uniqueCount="240">
   <si>
     <t>variant ID</t>
   </si>
@@ -291,6 +291,9 @@
     <t>chimeras in AC alt (all tiers)</t>
   </si>
   <si>
+    <t>chimera-corrected cvrg</t>
+  </si>
+  <si>
     <t>chimera-corrected AF (all tiers)</t>
   </si>
   <si>
@@ -304,6 +307,9 @@
   </si>
   <si>
     <t>chimeras in AC alt (tiers 1.1-2.4)</t>
+  </si>
+  <si>
+    <t>chimera-corrected cvrg (tiers 1.1-2.4)</t>
   </si>
   <si>
     <t>chimera-corrected AF (tiers 1.1-2.4)</t>
@@ -17379,13 +17385,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AH4"/>
+  <dimension ref="A1:AJ4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:36">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -17488,8 +17494,14 @@
       <c r="AH1" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="2" spans="1:34">
+      <c r="AI1" t="s">
+        <v>120</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -17506,53 +17518,53 @@
         <v>0</v>
       </c>
       <c r="F2">
+        <v>61</v>
+      </c>
+      <c r="G2">
         <v>0.6229508196721312</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>61</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>38</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>0.6229508196721312</v>
       </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
       <c r="K2">
-        <v>0.6229508196721312</v>
+        <v>0</v>
       </c>
       <c r="L2">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="M2">
         <v>0.6229508196721312</v>
       </c>
       <c r="N2">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="O2">
-        <v>0</v>
+        <v>0.6229508196721312</v>
       </c>
       <c r="P2">
         <v>0</v>
       </c>
       <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
         <v>32</v>
       </c>
-      <c r="R2">
-        <v>0</v>
-      </c>
-      <c r="S2">
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
         <v>6</v>
       </c>
-      <c r="T2">
-        <v>0</v>
-      </c>
-      <c r="U2">
-        <v>0</v>
-      </c>
       <c r="V2">
         <v>0</v>
       </c>
@@ -17569,16 +17581,16 @@
         <v>0</v>
       </c>
       <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
         <v>0.5245901639344263</v>
       </c>
-      <c r="AB2">
+      <c r="AD2">
         <v>0.5245901639344263</v>
-      </c>
-      <c r="AC2">
-        <v>0.6229508196721312</v>
-      </c>
-      <c r="AD2">
-        <v>0.6229508196721312</v>
       </c>
       <c r="AE2">
         <v>0.6229508196721312</v>
@@ -17592,8 +17604,14 @@
       <c r="AH2">
         <v>0.6229508196721312</v>
       </c>
-    </row>
-    <row r="3" spans="1:34">
+      <c r="AI2">
+        <v>0.6229508196721312</v>
+      </c>
+      <c r="AJ2">
+        <v>0.6229508196721312</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36">
       <c r="A3" t="s">
         <v>77</v>
       </c>
@@ -17610,53 +17628,53 @@
         <v>0</v>
       </c>
       <c r="F3">
+        <v>61</v>
+      </c>
+      <c r="G3">
         <v>0.6065573770491803</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>61</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>37</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>0.6065573770491803</v>
       </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
       <c r="K3">
-        <v>0.6065573770491803</v>
+        <v>0</v>
       </c>
       <c r="L3">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="M3">
         <v>0.6065573770491803</v>
       </c>
       <c r="N3">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="O3">
-        <v>0</v>
+        <v>0.6065573770491803</v>
       </c>
       <c r="P3">
         <v>0</v>
       </c>
       <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
         <v>34</v>
       </c>
-      <c r="R3">
-        <v>0</v>
-      </c>
-      <c r="S3">
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
         <v>3</v>
       </c>
-      <c r="T3">
-        <v>0</v>
-      </c>
-      <c r="U3">
-        <v>0</v>
-      </c>
       <c r="V3">
         <v>0</v>
       </c>
@@ -17673,16 +17691,16 @@
         <v>0</v>
       </c>
       <c r="AA3">
+        <v>0</v>
+      </c>
+      <c r="AB3">
+        <v>0</v>
+      </c>
+      <c r="AC3">
         <v>0.5573770491803278</v>
       </c>
-      <c r="AB3">
+      <c r="AD3">
         <v>0.5573770491803278</v>
-      </c>
-      <c r="AC3">
-        <v>0.6065573770491803</v>
-      </c>
-      <c r="AD3">
-        <v>0.6065573770491803</v>
       </c>
       <c r="AE3">
         <v>0.6065573770491803</v>
@@ -17696,8 +17714,14 @@
       <c r="AH3">
         <v>0.6065573770491803</v>
       </c>
-    </row>
-    <row r="4" spans="1:34">
+      <c r="AI3">
+        <v>0.6065573770491803</v>
+      </c>
+      <c r="AJ3">
+        <v>0.6065573770491803</v>
+      </c>
+    </row>
+    <row r="4" spans="1:36">
       <c r="A4" t="s">
         <v>79</v>
       </c>
@@ -17714,34 +17738,34 @@
         <v>0</v>
       </c>
       <c r="F4">
+        <v>12</v>
+      </c>
+      <c r="G4">
         <v>0.5833333333333334</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>12</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>7</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>0.5833333333333334</v>
       </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
       <c r="K4">
-        <v>0.5833333333333334</v>
+        <v>0</v>
       </c>
       <c r="L4">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="M4">
         <v>0.5833333333333334</v>
       </c>
       <c r="N4">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="O4">
-        <v>0</v>
+        <v>0.5833333333333334</v>
       </c>
       <c r="P4">
         <v>0</v>
@@ -17753,14 +17777,14 @@
         <v>0</v>
       </c>
       <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
         <v>7</v>
       </c>
-      <c r="T4">
-        <v>0</v>
-      </c>
-      <c r="U4">
-        <v>0</v>
-      </c>
       <c r="V4">
         <v>0</v>
       </c>
@@ -17783,10 +17807,10 @@
         <v>0</v>
       </c>
       <c r="AC4">
-        <v>0.5833333333333334</v>
+        <v>0</v>
       </c>
       <c r="AD4">
-        <v>0.5833333333333334</v>
+        <v>0</v>
       </c>
       <c r="AE4">
         <v>0.5833333333333334</v>
@@ -17800,51 +17824,57 @@
       <c r="AH4">
         <v>0.5833333333333334</v>
       </c>
+      <c r="AI4">
+        <v>0.5833333333333334</v>
+      </c>
+      <c r="AJ4">
+        <v>0.5833333333333334</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="N2:O2 N1:O1">
+  <conditionalFormatting sqref="P2:Q2 P1:Q1">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>$N$1="tier 1.1"</formula>
+      <formula>$P$1="tier 1.1"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N3:O3 N1:O1">
+  <conditionalFormatting sqref="P3:Q3 P1:Q1">
     <cfRule type="expression" dxfId="0" priority="4">
-      <formula>$N$1="tier 1.1"</formula>
+      <formula>$P$1="tier 1.1"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N4:O4 N1:O1">
+  <conditionalFormatting sqref="P4:Q4 P1:Q1">
     <cfRule type="expression" dxfId="0" priority="7">
-      <formula>$N$1="tier 1.1"</formula>
+      <formula>$P$1="tier 1.1"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P2:S2 P1:S1">
+  <conditionalFormatting sqref="R2:U2 R1:U1">
     <cfRule type="expression" dxfId="1" priority="2">
-      <formula>$P$1="tier 2.1"</formula>
+      <formula>$R$1="tier 2.1"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P3:S3 P1:S1">
+  <conditionalFormatting sqref="R3:U3 R1:U1">
     <cfRule type="expression" dxfId="1" priority="5">
-      <formula>$P$1="tier 2.1"</formula>
+      <formula>$R$1="tier 2.1"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P4:S4 P1:S1">
+  <conditionalFormatting sqref="R4:U4 R1:U1">
     <cfRule type="expression" dxfId="1" priority="8">
-      <formula>$P$1="tier 2.1"</formula>
+      <formula>$R$1="tier 2.1"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T2:X2 T1:X1">
+  <conditionalFormatting sqref="V2:Z2 V1:Z1">
     <cfRule type="expression" dxfId="2" priority="3">
-      <formula>$T$1="tier 3.1"</formula>
+      <formula>$V$1="tier 3.1"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T3:X3 T1:X1">
+  <conditionalFormatting sqref="V3:Z3 V1:Z1">
     <cfRule type="expression" dxfId="2" priority="6">
-      <formula>$T$1="tier 3.1"</formula>
+      <formula>$V$1="tier 3.1"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T4:X4 T1:X1">
+  <conditionalFormatting sqref="V4:Z4 V1:Z1">
     <cfRule type="expression" dxfId="2" priority="9">
-      <formula>$T$1="tier 3.1"</formula>
+      <formula>$V$1="tier 3.1"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17864,12 +17894,12 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -17877,7 +17907,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -17885,7 +17915,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -17893,7 +17923,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B5">
         <v>66</v>
@@ -17901,7 +17931,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -17909,7 +17939,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B7">
         <v>16</v>
@@ -17917,7 +17947,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -17925,7 +17955,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -17933,7 +17963,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -17941,7 +17971,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -17949,7 +17979,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -17957,7 +17987,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17" spans="1:33">
@@ -18063,2163 +18093,2163 @@
     </row>
     <row r="19" spans="1:33">
       <c r="A19" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B19" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20" spans="1:33">
       <c r="A20" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B20" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C20" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D20" t="s">
         <v>36</v>
       </c>
       <c r="E20" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F20" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="G20" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="H20" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="I20" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="J20" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="K20" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="L20" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="M20" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="N20" t="s">
+        <v>136</v>
+      </c>
+      <c r="O20" t="s">
+        <v>136</v>
+      </c>
+      <c r="P20" t="s">
         <v>134</v>
       </c>
-      <c r="O20" t="s">
-        <v>134</v>
-      </c>
-      <c r="P20" t="s">
-        <v>132</v>
-      </c>
       <c r="Q20" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="R20" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="S20" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="T20" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="U20" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="V20" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="W20" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="X20" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="Y20" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="Z20" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="AA20" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="AB20" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AC20" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AD20" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="AE20" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="21" spans="1:33">
       <c r="C21" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D21" t="s">
         <v>38</v>
       </c>
       <c r="I21" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="J21" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="K21" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="L21" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="M21" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="N21" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="O21" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="P21" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="Q21" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="V21" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="W21" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="X21" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="Y21" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="Z21" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="AA21" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="AB21" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AC21" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AD21" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="AE21" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="24" spans="1:33">
       <c r="A24" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B24" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C24" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D24" t="s">
         <v>36</v>
       </c>
       <c r="E24" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F24" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="G24" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="H24" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="I24" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="J24" t="s">
+        <v>143</v>
+      </c>
+      <c r="K24" t="s">
+        <v>144</v>
+      </c>
+      <c r="L24" t="s">
+        <v>143</v>
+      </c>
+      <c r="M24" t="s">
+        <v>144</v>
+      </c>
+      <c r="N24" t="s">
+        <v>136</v>
+      </c>
+      <c r="O24" t="s">
+        <v>136</v>
+      </c>
+      <c r="P24" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>144</v>
+      </c>
+      <c r="R24" t="s">
+        <v>136</v>
+      </c>
+      <c r="S24" t="s">
+        <v>136</v>
+      </c>
+      <c r="T24" t="s">
+        <v>137</v>
+      </c>
+      <c r="U24" t="s">
+        <v>137</v>
+      </c>
+      <c r="V24" t="s">
+        <v>136</v>
+      </c>
+      <c r="W24" t="s">
+        <v>136</v>
+      </c>
+      <c r="X24" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>136</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>136</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>136</v>
+      </c>
+      <c r="AB24" t="s">
+        <v>138</v>
+      </c>
+      <c r="AC24" t="s">
+        <v>139</v>
+      </c>
+      <c r="AD24" t="s">
+        <v>140</v>
+      </c>
+      <c r="AE24" t="s">
         <v>141</v>
-      </c>
-      <c r="K24" t="s">
-        <v>142</v>
-      </c>
-      <c r="L24" t="s">
-        <v>141</v>
-      </c>
-      <c r="M24" t="s">
-        <v>142</v>
-      </c>
-      <c r="N24" t="s">
-        <v>134</v>
-      </c>
-      <c r="O24" t="s">
-        <v>134</v>
-      </c>
-      <c r="P24" t="s">
-        <v>141</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>142</v>
-      </c>
-      <c r="R24" t="s">
-        <v>134</v>
-      </c>
-      <c r="S24" t="s">
-        <v>134</v>
-      </c>
-      <c r="T24" t="s">
-        <v>135</v>
-      </c>
-      <c r="U24" t="s">
-        <v>135</v>
-      </c>
-      <c r="V24" t="s">
-        <v>134</v>
-      </c>
-      <c r="W24" t="s">
-        <v>134</v>
-      </c>
-      <c r="X24" t="s">
-        <v>134</v>
-      </c>
-      <c r="Y24" t="s">
-        <v>134</v>
-      </c>
-      <c r="Z24" t="s">
-        <v>134</v>
-      </c>
-      <c r="AA24" t="s">
-        <v>134</v>
-      </c>
-      <c r="AB24" t="s">
-        <v>136</v>
-      </c>
-      <c r="AC24" t="s">
-        <v>137</v>
-      </c>
-      <c r="AD24" t="s">
-        <v>138</v>
-      </c>
-      <c r="AE24" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="25" spans="1:33">
       <c r="C25" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D25" t="s">
         <v>38</v>
       </c>
       <c r="E25" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="F25" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="G25" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H25" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="I25" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="J25" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="K25" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="L25" t="s">
+        <v>141</v>
+      </c>
+      <c r="M25" t="s">
+        <v>149</v>
+      </c>
+      <c r="N25" t="s">
+        <v>136</v>
+      </c>
+      <c r="O25" t="s">
+        <v>136</v>
+      </c>
+      <c r="P25" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>149</v>
+      </c>
+      <c r="R25" t="s">
+        <v>136</v>
+      </c>
+      <c r="S25" t="s">
+        <v>136</v>
+      </c>
+      <c r="T25" t="s">
+        <v>137</v>
+      </c>
+      <c r="U25" t="s">
+        <v>137</v>
+      </c>
+      <c r="V25" t="s">
+        <v>136</v>
+      </c>
+      <c r="W25" t="s">
+        <v>136</v>
+      </c>
+      <c r="X25" t="s">
+        <v>137</v>
+      </c>
+      <c r="Y25" t="s">
+        <v>150</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>136</v>
+      </c>
+      <c r="AA25" t="s">
+        <v>136</v>
+      </c>
+      <c r="AB25" t="s">
+        <v>138</v>
+      </c>
+      <c r="AC25" t="s">
         <v>139</v>
       </c>
-      <c r="M25" t="s">
-        <v>147</v>
-      </c>
-      <c r="N25" t="s">
-        <v>134</v>
-      </c>
-      <c r="O25" t="s">
-        <v>134</v>
-      </c>
-      <c r="P25" t="s">
-        <v>139</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>147</v>
-      </c>
-      <c r="R25" t="s">
-        <v>134</v>
-      </c>
-      <c r="S25" t="s">
-        <v>134</v>
-      </c>
-      <c r="T25" t="s">
-        <v>135</v>
-      </c>
-      <c r="U25" t="s">
-        <v>135</v>
-      </c>
-      <c r="V25" t="s">
-        <v>134</v>
-      </c>
-      <c r="W25" t="s">
-        <v>134</v>
-      </c>
-      <c r="X25" t="s">
-        <v>135</v>
-      </c>
-      <c r="Y25" t="s">
-        <v>148</v>
-      </c>
-      <c r="Z25" t="s">
-        <v>134</v>
-      </c>
-      <c r="AA25" t="s">
-        <v>134</v>
-      </c>
-      <c r="AB25" t="s">
-        <v>136</v>
-      </c>
-      <c r="AC25" t="s">
-        <v>137</v>
-      </c>
       <c r="AD25" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="AE25" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="27" spans="1:33">
       <c r="A27" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B27" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="28" spans="1:33">
       <c r="A28" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B28" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C28" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D28" t="s">
         <v>36</v>
       </c>
       <c r="E28" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="F28" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="G28" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="H28" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="I28" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="J28" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="K28" t="s">
+        <v>137</v>
+      </c>
+      <c r="L28" t="s">
+        <v>158</v>
+      </c>
+      <c r="M28" t="s">
+        <v>137</v>
+      </c>
+      <c r="N28" t="s">
+        <v>136</v>
+      </c>
+      <c r="O28" t="s">
+        <v>136</v>
+      </c>
+      <c r="P28" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>137</v>
+      </c>
+      <c r="R28" t="s">
+        <v>136</v>
+      </c>
+      <c r="S28" t="s">
+        <v>136</v>
+      </c>
+      <c r="T28" t="s">
+        <v>137</v>
+      </c>
+      <c r="U28" t="s">
+        <v>137</v>
+      </c>
+      <c r="V28" t="s">
+        <v>136</v>
+      </c>
+      <c r="W28" t="s">
+        <v>136</v>
+      </c>
+      <c r="X28" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y28" t="s">
+        <v>136</v>
+      </c>
+      <c r="Z28" t="s">
+        <v>136</v>
+      </c>
+      <c r="AA28" t="s">
+        <v>136</v>
+      </c>
+      <c r="AB28" t="s">
+        <v>137</v>
+      </c>
+      <c r="AC28" t="s">
         <v>135</v>
       </c>
-      <c r="L28" t="s">
-        <v>156</v>
-      </c>
-      <c r="M28" t="s">
-        <v>135</v>
-      </c>
-      <c r="N28" t="s">
-        <v>134</v>
-      </c>
-      <c r="O28" t="s">
-        <v>134</v>
-      </c>
-      <c r="P28" t="s">
-        <v>156</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>135</v>
-      </c>
-      <c r="R28" t="s">
-        <v>134</v>
-      </c>
-      <c r="S28" t="s">
-        <v>134</v>
-      </c>
-      <c r="T28" t="s">
-        <v>135</v>
-      </c>
-      <c r="U28" t="s">
-        <v>135</v>
-      </c>
-      <c r="V28" t="s">
-        <v>134</v>
-      </c>
-      <c r="W28" t="s">
-        <v>134</v>
-      </c>
-      <c r="X28" t="s">
-        <v>134</v>
-      </c>
-      <c r="Y28" t="s">
-        <v>134</v>
-      </c>
-      <c r="Z28" t="s">
-        <v>134</v>
-      </c>
-      <c r="AA28" t="s">
-        <v>134</v>
-      </c>
-      <c r="AB28" t="s">
-        <v>135</v>
-      </c>
-      <c r="AC28" t="s">
-        <v>133</v>
-      </c>
       <c r="AD28" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="AE28" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="29" spans="1:33">
       <c r="C29" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D29" t="s">
         <v>38</v>
       </c>
       <c r="E29" t="s">
+        <v>161</v>
+      </c>
+      <c r="F29" t="s">
+        <v>156</v>
+      </c>
+      <c r="G29" t="s">
+        <v>162</v>
+      </c>
+      <c r="H29" t="s">
+        <v>163</v>
+      </c>
+      <c r="I29" t="s">
+        <v>157</v>
+      </c>
+      <c r="J29" t="s">
+        <v>158</v>
+      </c>
+      <c r="K29" t="s">
+        <v>137</v>
+      </c>
+      <c r="L29" t="s">
+        <v>158</v>
+      </c>
+      <c r="M29" t="s">
+        <v>137</v>
+      </c>
+      <c r="N29" t="s">
+        <v>136</v>
+      </c>
+      <c r="O29" t="s">
+        <v>136</v>
+      </c>
+      <c r="P29" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>137</v>
+      </c>
+      <c r="R29" t="s">
+        <v>136</v>
+      </c>
+      <c r="S29" t="s">
+        <v>136</v>
+      </c>
+      <c r="T29" t="s">
+        <v>137</v>
+      </c>
+      <c r="U29" t="s">
+        <v>137</v>
+      </c>
+      <c r="V29" t="s">
+        <v>136</v>
+      </c>
+      <c r="W29" t="s">
+        <v>136</v>
+      </c>
+      <c r="X29" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y29" t="s">
+        <v>136</v>
+      </c>
+      <c r="Z29" t="s">
+        <v>136</v>
+      </c>
+      <c r="AA29" t="s">
+        <v>136</v>
+      </c>
+      <c r="AB29" t="s">
+        <v>137</v>
+      </c>
+      <c r="AC29" t="s">
+        <v>135</v>
+      </c>
+      <c r="AD29" t="s">
         <v>159</v>
       </c>
-      <c r="F29" t="s">
-        <v>154</v>
-      </c>
-      <c r="G29" t="s">
+      <c r="AE29" t="s">
         <v>160</v>
-      </c>
-      <c r="H29" t="s">
-        <v>161</v>
-      </c>
-      <c r="I29" t="s">
-        <v>155</v>
-      </c>
-      <c r="J29" t="s">
-        <v>156</v>
-      </c>
-      <c r="K29" t="s">
-        <v>135</v>
-      </c>
-      <c r="L29" t="s">
-        <v>156</v>
-      </c>
-      <c r="M29" t="s">
-        <v>135</v>
-      </c>
-      <c r="N29" t="s">
-        <v>134</v>
-      </c>
-      <c r="O29" t="s">
-        <v>134</v>
-      </c>
-      <c r="P29" t="s">
-        <v>156</v>
-      </c>
-      <c r="Q29" t="s">
-        <v>135</v>
-      </c>
-      <c r="R29" t="s">
-        <v>134</v>
-      </c>
-      <c r="S29" t="s">
-        <v>134</v>
-      </c>
-      <c r="T29" t="s">
-        <v>135</v>
-      </c>
-      <c r="U29" t="s">
-        <v>135</v>
-      </c>
-      <c r="V29" t="s">
-        <v>134</v>
-      </c>
-      <c r="W29" t="s">
-        <v>134</v>
-      </c>
-      <c r="X29" t="s">
-        <v>134</v>
-      </c>
-      <c r="Y29" t="s">
-        <v>134</v>
-      </c>
-      <c r="Z29" t="s">
-        <v>134</v>
-      </c>
-      <c r="AA29" t="s">
-        <v>134</v>
-      </c>
-      <c r="AB29" t="s">
-        <v>135</v>
-      </c>
-      <c r="AC29" t="s">
-        <v>133</v>
-      </c>
-      <c r="AD29" t="s">
-        <v>157</v>
-      </c>
-      <c r="AE29" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="31" spans="1:33">
       <c r="A31" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B31" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="32" spans="1:33">
       <c r="A32" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B32" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C32" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D32" t="s">
         <v>36</v>
       </c>
       <c r="E32" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="F32" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="G32" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="H32" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="I32" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="J32" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="K32" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="L32" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="M32" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="N32" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="O32" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="P32" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="Q32" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="R32" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="S32" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="T32" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="U32" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="V32" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="W32" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="X32" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="Y32" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="Z32" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="AA32" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="AB32" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AC32" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AD32" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="AE32" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="33" spans="1:31">
       <c r="C33" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D33" t="s">
         <v>38</v>
       </c>
       <c r="I33" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="J33" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="K33" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="L33" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="M33" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="N33" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="O33" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="P33" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="Q33" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="V33" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="W33" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="X33" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="Y33" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="Z33" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="AA33" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="AB33" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AC33" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AD33" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="AE33" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="35" spans="1:31">
       <c r="A35" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B35" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="36" spans="1:31">
       <c r="A36" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B36" t="s">
         <v>34</v>
       </c>
       <c r="C36" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D36" t="s">
         <v>36</v>
       </c>
       <c r="E36" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="F36" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G36" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="H36" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="I36" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="J36" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="K36" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="L36" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="M36" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="N36" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="O36" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="P36" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="Q36" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="R36" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="S36" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="T36" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="U36" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="V36" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="W36" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="X36" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="Y36" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="Z36" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="AA36" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="AB36" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AC36" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AD36" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="AE36" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="37" spans="1:31">
       <c r="C37" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D37" t="s">
         <v>38</v>
       </c>
       <c r="E37" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="F37" t="s">
+        <v>178</v>
+      </c>
+      <c r="G37" t="s">
         <v>176</v>
       </c>
-      <c r="G37" t="s">
-        <v>174</v>
-      </c>
       <c r="H37" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="I37" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="J37" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="K37" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="L37" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="M37" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="N37" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="O37" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="P37" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="Q37" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="R37" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="S37" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="T37" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="U37" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="V37" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="W37" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="X37" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="Y37" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="Z37" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="AA37" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="AB37" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AC37" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AD37" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="AE37" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="39" spans="1:31">
       <c r="A39" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B39" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="40" spans="1:31">
       <c r="A40" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B40" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C40" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="D40" t="s">
         <v>36</v>
       </c>
       <c r="I40" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="J40" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="K40" t="s">
+        <v>140</v>
+      </c>
+      <c r="L40" t="s">
+        <v>136</v>
+      </c>
+      <c r="M40" t="s">
+        <v>140</v>
+      </c>
+      <c r="N40" t="s">
+        <v>136</v>
+      </c>
+      <c r="O40" t="s">
+        <v>136</v>
+      </c>
+      <c r="P40" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>140</v>
+      </c>
+      <c r="U40" t="s">
+        <v>137</v>
+      </c>
+      <c r="V40" t="s">
+        <v>136</v>
+      </c>
+      <c r="W40" t="s">
+        <v>136</v>
+      </c>
+      <c r="X40" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y40" t="s">
+        <v>136</v>
+      </c>
+      <c r="Z40" t="s">
+        <v>136</v>
+      </c>
+      <c r="AA40" t="s">
+        <v>136</v>
+      </c>
+      <c r="AB40" t="s">
         <v>138</v>
       </c>
-      <c r="L40" t="s">
-        <v>134</v>
-      </c>
-      <c r="M40" t="s">
-        <v>138</v>
-      </c>
-      <c r="N40" t="s">
-        <v>134</v>
-      </c>
-      <c r="O40" t="s">
-        <v>134</v>
-      </c>
-      <c r="P40" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q40" t="s">
-        <v>138</v>
-      </c>
-      <c r="U40" t="s">
-        <v>135</v>
-      </c>
-      <c r="V40" t="s">
-        <v>134</v>
-      </c>
-      <c r="W40" t="s">
-        <v>134</v>
-      </c>
-      <c r="X40" t="s">
-        <v>134</v>
-      </c>
-      <c r="Y40" t="s">
-        <v>134</v>
-      </c>
-      <c r="Z40" t="s">
-        <v>134</v>
-      </c>
-      <c r="AA40" t="s">
-        <v>134</v>
-      </c>
-      <c r="AB40" t="s">
-        <v>136</v>
-      </c>
       <c r="AC40" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AD40" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="AE40" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="41" spans="1:31">
       <c r="C41" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="D41" t="s">
         <v>38</v>
       </c>
       <c r="E41" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="F41" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="G41" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="H41" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="I41" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="J41" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="K41" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="L41" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="M41" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="N41" t="s">
+        <v>136</v>
+      </c>
+      <c r="O41" t="s">
+        <v>136</v>
+      </c>
+      <c r="P41" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q41" t="s">
         <v>134</v>
       </c>
-      <c r="O41" t="s">
-        <v>134</v>
-      </c>
-      <c r="P41" t="s">
-        <v>135</v>
-      </c>
-      <c r="Q41" t="s">
-        <v>132</v>
-      </c>
       <c r="R41" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="S41" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="T41" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="U41" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="V41" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="W41" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="X41" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="Y41" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="Z41" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="AA41" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="AB41" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AC41" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AD41" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="AE41" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="43" spans="1:31">
       <c r="A43" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B43" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="44" spans="1:31">
       <c r="A44" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B44" t="s">
         <v>44</v>
       </c>
       <c r="C44" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="D44" t="s">
         <v>36</v>
       </c>
       <c r="E44" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="F44" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="G44" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="H44" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="I44" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="J44" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="K44" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="L44" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="M44" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="N44" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="O44" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="P44" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="Q44" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="R44" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="S44" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="T44" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="U44" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="V44" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="W44" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="X44" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="Y44" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="Z44" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="AA44" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="AB44" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AC44" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AD44" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="AE44" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="45" spans="1:31">
       <c r="C45" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="D45" t="s">
         <v>38</v>
       </c>
       <c r="E45" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="F45" t="s">
+        <v>178</v>
+      </c>
+      <c r="G45" t="s">
         <v>176</v>
       </c>
-      <c r="G45" t="s">
-        <v>174</v>
-      </c>
       <c r="H45" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="I45" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="J45" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="K45" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="L45" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="M45" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="N45" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="O45" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="P45" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="Q45" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="R45" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="S45" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="T45" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="U45" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="V45" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="W45" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="X45" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="Y45" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="Z45" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="AA45" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="AB45" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AC45" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AD45" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="AE45" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="47" spans="1:31">
       <c r="A47" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B47" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="48" spans="1:31">
       <c r="A48" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B48" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C48" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="D48" t="s">
         <v>36</v>
       </c>
       <c r="E48" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="F48" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="G48" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="H48" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="I48" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="J48" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="K48" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="L48" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="M48" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="N48" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="O48" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="P48" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>137</v>
+      </c>
+      <c r="R48" t="s">
+        <v>137</v>
+      </c>
+      <c r="S48" t="s">
+        <v>196</v>
+      </c>
+      <c r="T48" t="s">
+        <v>136</v>
+      </c>
+      <c r="U48" t="s">
+        <v>196</v>
+      </c>
+      <c r="V48" t="s">
+        <v>136</v>
+      </c>
+      <c r="W48" t="s">
+        <v>136</v>
+      </c>
+      <c r="X48" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y48" t="s">
+        <v>137</v>
+      </c>
+      <c r="Z48" t="s">
+        <v>136</v>
+      </c>
+      <c r="AA48" t="s">
+        <v>136</v>
+      </c>
+      <c r="AB48" t="s">
         <v>134</v>
       </c>
-      <c r="Q48" t="s">
-        <v>135</v>
-      </c>
-      <c r="R48" t="s">
-        <v>135</v>
-      </c>
-      <c r="S48" t="s">
-        <v>194</v>
-      </c>
-      <c r="T48" t="s">
+      <c r="AC48" t="s">
         <v>134</v>
       </c>
-      <c r="U48" t="s">
-        <v>194</v>
-      </c>
-      <c r="V48" t="s">
-        <v>134</v>
-      </c>
-      <c r="W48" t="s">
-        <v>134</v>
-      </c>
-      <c r="X48" t="s">
-        <v>134</v>
-      </c>
-      <c r="Y48" t="s">
-        <v>135</v>
-      </c>
-      <c r="Z48" t="s">
-        <v>134</v>
-      </c>
-      <c r="AA48" t="s">
-        <v>134</v>
-      </c>
-      <c r="AB48" t="s">
-        <v>132</v>
-      </c>
-      <c r="AC48" t="s">
-        <v>132</v>
-      </c>
       <c r="AD48" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="AE48" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="49" spans="1:31">
       <c r="C49" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="D49" t="s">
         <v>38</v>
       </c>
       <c r="F49" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="H49" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="I49" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="J49" t="s">
+        <v>136</v>
+      </c>
+      <c r="K49" t="s">
         <v>134</v>
       </c>
-      <c r="K49" t="s">
-        <v>132</v>
-      </c>
       <c r="L49" t="s">
+        <v>136</v>
+      </c>
+      <c r="M49" t="s">
+        <v>170</v>
+      </c>
+      <c r="N49" t="s">
+        <v>136</v>
+      </c>
+      <c r="O49" t="s">
+        <v>137</v>
+      </c>
+      <c r="P49" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>137</v>
+      </c>
+      <c r="S49" t="s">
+        <v>196</v>
+      </c>
+      <c r="U49" t="s">
+        <v>196</v>
+      </c>
+      <c r="V49" t="s">
+        <v>136</v>
+      </c>
+      <c r="W49" t="s">
+        <v>136</v>
+      </c>
+      <c r="X49" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y49" t="s">
+        <v>137</v>
+      </c>
+      <c r="Z49" t="s">
+        <v>136</v>
+      </c>
+      <c r="AA49" t="s">
+        <v>136</v>
+      </c>
+      <c r="AB49" t="s">
         <v>134</v>
       </c>
-      <c r="M49" t="s">
-        <v>168</v>
-      </c>
-      <c r="N49" t="s">
+      <c r="AC49" t="s">
         <v>134</v>
       </c>
-      <c r="O49" t="s">
-        <v>135</v>
-      </c>
-      <c r="P49" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q49" t="s">
-        <v>135</v>
-      </c>
-      <c r="S49" t="s">
-        <v>194</v>
-      </c>
-      <c r="U49" t="s">
-        <v>194</v>
-      </c>
-      <c r="V49" t="s">
-        <v>134</v>
-      </c>
-      <c r="W49" t="s">
-        <v>134</v>
-      </c>
-      <c r="X49" t="s">
-        <v>134</v>
-      </c>
-      <c r="Y49" t="s">
-        <v>135</v>
-      </c>
-      <c r="Z49" t="s">
-        <v>134</v>
-      </c>
-      <c r="AA49" t="s">
-        <v>134</v>
-      </c>
-      <c r="AB49" t="s">
-        <v>132</v>
-      </c>
-      <c r="AC49" t="s">
-        <v>132</v>
-      </c>
       <c r="AD49" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="AE49" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="51" spans="1:31">
       <c r="A51" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B51" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="52" spans="1:31">
       <c r="A52" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B52" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C52" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="D52" t="s">
         <v>36</v>
       </c>
       <c r="E52" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="F52" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="G52" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="H52" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="I52" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="J52" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="K52" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="L52" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="M52" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="N52" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="O52" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="P52" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="Q52" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="R52" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="S52" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="T52" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="U52" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="V52" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="W52" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="X52" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="Y52" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="Z52" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="AA52" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="AB52" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="AC52" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="AD52" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="AE52" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="53" spans="1:31">
       <c r="C53" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="D53" t="s">
         <v>38</v>
       </c>
       <c r="E53" t="s">
+        <v>210</v>
+      </c>
+      <c r="F53" t="s">
+        <v>210</v>
+      </c>
+      <c r="G53" t="s">
+        <v>204</v>
+      </c>
+      <c r="H53" t="s">
+        <v>211</v>
+      </c>
+      <c r="I53" t="s">
+        <v>205</v>
+      </c>
+      <c r="J53" t="s">
+        <v>170</v>
+      </c>
+      <c r="K53" t="s">
+        <v>134</v>
+      </c>
+      <c r="L53" t="s">
+        <v>170</v>
+      </c>
+      <c r="M53" t="s">
+        <v>134</v>
+      </c>
+      <c r="N53" t="s">
+        <v>136</v>
+      </c>
+      <c r="O53" t="s">
+        <v>137</v>
+      </c>
+      <c r="P53" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q53" t="s">
+        <v>170</v>
+      </c>
+      <c r="R53" t="s">
+        <v>136</v>
+      </c>
+      <c r="S53" t="s">
+        <v>206</v>
+      </c>
+      <c r="T53" t="s">
+        <v>137</v>
+      </c>
+      <c r="U53" t="s">
+        <v>207</v>
+      </c>
+      <c r="V53" t="s">
+        <v>136</v>
+      </c>
+      <c r="W53" t="s">
+        <v>136</v>
+      </c>
+      <c r="X53" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y53" t="s">
+        <v>136</v>
+      </c>
+      <c r="Z53" t="s">
+        <v>136</v>
+      </c>
+      <c r="AA53" t="s">
+        <v>136</v>
+      </c>
+      <c r="AB53" t="s">
+        <v>137</v>
+      </c>
+      <c r="AC53" t="s">
+        <v>137</v>
+      </c>
+      <c r="AD53" t="s">
         <v>208</v>
       </c>
-      <c r="F53" t="s">
-        <v>208</v>
-      </c>
-      <c r="G53" t="s">
-        <v>202</v>
-      </c>
-      <c r="H53" t="s">
+      <c r="AE53" t="s">
         <v>209</v>
-      </c>
-      <c r="I53" t="s">
-        <v>203</v>
-      </c>
-      <c r="J53" t="s">
-        <v>168</v>
-      </c>
-      <c r="K53" t="s">
-        <v>132</v>
-      </c>
-      <c r="L53" t="s">
-        <v>168</v>
-      </c>
-      <c r="M53" t="s">
-        <v>132</v>
-      </c>
-      <c r="N53" t="s">
-        <v>134</v>
-      </c>
-      <c r="O53" t="s">
-        <v>135</v>
-      </c>
-      <c r="P53" t="s">
-        <v>168</v>
-      </c>
-      <c r="Q53" t="s">
-        <v>168</v>
-      </c>
-      <c r="R53" t="s">
-        <v>134</v>
-      </c>
-      <c r="S53" t="s">
-        <v>204</v>
-      </c>
-      <c r="T53" t="s">
-        <v>135</v>
-      </c>
-      <c r="U53" t="s">
-        <v>205</v>
-      </c>
-      <c r="V53" t="s">
-        <v>134</v>
-      </c>
-      <c r="W53" t="s">
-        <v>134</v>
-      </c>
-      <c r="X53" t="s">
-        <v>134</v>
-      </c>
-      <c r="Y53" t="s">
-        <v>134</v>
-      </c>
-      <c r="Z53" t="s">
-        <v>134</v>
-      </c>
-      <c r="AA53" t="s">
-        <v>134</v>
-      </c>
-      <c r="AB53" t="s">
-        <v>135</v>
-      </c>
-      <c r="AC53" t="s">
-        <v>135</v>
-      </c>
-      <c r="AD53" t="s">
-        <v>206</v>
-      </c>
-      <c r="AE53" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="55" spans="1:31">
       <c r="A55" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="B55" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="56" spans="1:31">
       <c r="A56" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B56" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="C56" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="D56" t="s">
         <v>36</v>
       </c>
       <c r="E56" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F56" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="G56" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="H56" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="I56" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="J56" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="K56" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="L56" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="M56" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="N56" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="O56" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="P56" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="Q56" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="R56" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="S56" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="T56" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="U56" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="V56" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="W56" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="X56" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="Y56" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="Z56" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="AA56" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="AB56" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="AC56" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="AD56" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="AE56" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="57" spans="1:31">
       <c r="C57" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="D57" t="s">
         <v>38</v>
       </c>
       <c r="I57" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="J57" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="K57" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="L57" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="M57" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="N57" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="O57" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="P57" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="Q57" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="V57" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="W57" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="X57" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="Y57" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="Z57" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="AA57" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="AB57" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="AC57" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="AD57" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="AE57" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="59" spans="1:31">
       <c r="A59" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B59" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="60" spans="1:31">
       <c r="A60" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B60" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="C60" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="D60" t="s">
         <v>36</v>
       </c>
       <c r="E60" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="F60" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="G60" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="H60" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="I60" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="J60" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="K60" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="L60" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="M60" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="N60" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="O60" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="P60" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="Q60" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="R60" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="S60" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="T60" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="U60" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="V60" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="W60" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="X60" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="Y60" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="Z60" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="AA60" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="AB60" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="AC60" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="AD60" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="AE60" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="61" spans="1:31">
       <c r="C61" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="D61" t="s">
         <v>38</v>
       </c>
       <c r="E61" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="F61" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="G61" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="H61" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="I61" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="J61" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="K61" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="L61" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="M61" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="N61" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="O61" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="P61" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="Q61" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="R61" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="S61" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="T61" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="U61" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="V61" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="W61" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="X61" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="Y61" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="Z61" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="AA61" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="AB61" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="AC61" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="AD61" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="AE61" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="63" spans="1:31">
       <c r="A63" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B63" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="64" spans="1:31">
       <c r="A64" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B64" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C64" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D64" t="s">
         <v>36</v>
       </c>
       <c r="F64" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="H64" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="I64" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="J64" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="K64" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="L64" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="M64" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="N64" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="O64" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="P64" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="Q64" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="R64" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="S64" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="T64" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="U64" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="V64" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="W64" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="X64" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="Y64" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="Z64" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="AA64" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="AB64" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="AC64" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="AD64" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="AE64" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="65" spans="3:31">
       <c r="C65" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D65" t="s">
         <v>38</v>
       </c>
       <c r="I65" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="J65" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="K65" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="L65" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="M65" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="N65" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="O65" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="P65" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="Q65" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="V65" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="W65" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="X65" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="Y65" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="Z65" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="AA65" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="AB65" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="AC65" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="AD65" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="AE65" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>

</xml_diff>